<commit_message>
add diagram of my WS2812 measurement
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -3,27 +3,130 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BE7C50-24BE-41CB-B70A-26705A6D0538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148DF38A-3664-4978-AE0C-6D2C13C23360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{62C0D98D-7A85-4FDC-81DC-829BEE4BC2F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{62C0D98D-7A85-4FDC-81DC-829BEE4BC2F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Wavelength" sheetId="1" r:id="rId1"/>
+    <sheet name="WS2812D-F8" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Wavelength!$A$2:$A$7</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Wavelength!$B$1</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">Wavelength!$B$9:$B$26</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Wavelength!$A$9:$A$14</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Wavelength!$B$9:$B$14</definedName>
+    <definedName name="_xlchart.v1.100" hidden="1">'WS2812D-F8'!$A$6</definedName>
+    <definedName name="_xlchart.v1.101" hidden="1">'WS2812D-F8'!$B$2:$AK$2</definedName>
+    <definedName name="_xlchart.v1.102" hidden="1">'WS2812D-F8'!$B$2:$C$2</definedName>
+    <definedName name="_xlchart.v1.103" hidden="1">'WS2812D-F8'!$B$2:$J$2</definedName>
+    <definedName name="_xlchart.v1.104" hidden="1">'WS2812D-F8'!$B$3:$AK$3</definedName>
+    <definedName name="_xlchart.v1.105" hidden="1">'WS2812D-F8'!$B$3:$C$3</definedName>
+    <definedName name="_xlchart.v1.106" hidden="1">'WS2812D-F8'!$B$3:$J$3</definedName>
+    <definedName name="_xlchart.v1.107" hidden="1">'WS2812D-F8'!$B$4:$AK$4</definedName>
+    <definedName name="_xlchart.v1.108" hidden="1">'WS2812D-F8'!$B$4:$C$4</definedName>
+    <definedName name="_xlchart.v1.109" hidden="1">'WS2812D-F8'!$B$4:$J$4</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'WS2812D-F8'!#REF!</definedName>
+    <definedName name="_xlchart.v1.110" hidden="1">'WS2812D-F8'!$B$5:$AK$5</definedName>
+    <definedName name="_xlchart.v1.111" hidden="1">'WS2812D-F8'!$B$5:$C$5</definedName>
+    <definedName name="_xlchart.v1.112" hidden="1">'WS2812D-F8'!$B$5:$J$5</definedName>
+    <definedName name="_xlchart.v1.113" hidden="1">'WS2812D-F8'!$B$6:$AK$6</definedName>
+    <definedName name="_xlchart.v1.114" hidden="1">'WS2812D-F8'!$B$6:$J$6</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'WS2812D-F8'!$A$3</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'WS2812D-F8'!$A$3:$A$6</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'WS2812D-F8'!$A$4</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'WS2812D-F8'!$A$5</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'WS2812D-F8'!$A$6</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'WS2812D-F8'!$B$2:$AK$2</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'WS2812D-F8'!$B$2:$C$2</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'WS2812D-F8'!$B$2:$J$2</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Wavelength!$B$2:$B$7</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'WS2812D-F8'!$B$3:$AK$3</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'WS2812D-F8'!$B$3:$C$3</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'WS2812D-F8'!$B$3:$J$3</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'WS2812D-F8'!$B$4:$AK$4</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'WS2812D-F8'!$B$4:$C$4</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'WS2812D-F8'!$B$4:$J$4</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'WS2812D-F8'!$B$5:$AK$5</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'WS2812D-F8'!$B$5:$C$5</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'WS2812D-F8'!$B$5:$J$5</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'WS2812D-F8'!$B$6:$AK$6</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Wavelength!$C$1</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'WS2812D-F8'!$B$6:$J$6</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'WS2812D-F8'!#REF!</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'WS2812D-F8'!$A$3</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'WS2812D-F8'!$A$3:$A$6</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'WS2812D-F8'!$A$4</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'WS2812D-F8'!$A$5</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'WS2812D-F8'!$A$6</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'WS2812D-F8'!$B$2:$AK$2</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'WS2812D-F8'!$B$2:$C$2</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'WS2812D-F8'!$B$2:$J$2</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Wavelength!$C$2:$C$7</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">'WS2812D-F8'!$B$3:$AK$3</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">'WS2812D-F8'!$B$3:$C$3</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'WS2812D-F8'!$B$3:$J$3</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">'WS2812D-F8'!$B$4:$AK$4</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">'WS2812D-F8'!$B$4:$C$4</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">'WS2812D-F8'!$B$4:$J$4</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">'WS2812D-F8'!$B$5:$AK$5</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">'WS2812D-F8'!$B$5:$C$5</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">'WS2812D-F8'!$B$5:$J$5</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">'WS2812D-F8'!$B$6:$AK$6</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Wavelength!$D$1</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">'WS2812D-F8'!$B$6:$J$6</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">'WS2812D-F8'!$A$2</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">'WS2812D-F8'!$A$3</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">'WS2812D-F8'!$A$4</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">'WS2812D-F8'!$A$5</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">'WS2812D-F8'!$B$1:$E$1</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">'WS2812D-F8'!$B$2:$E$2</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">'WS2812D-F8'!$B$3:$E$3</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">'WS2812D-F8'!$B$4:$E$4</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">'WS2812D-F8'!$B$5:$E$5</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Wavelength!$D$2:$D$7</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">'WS2812D-F8'!#REF!</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">'WS2812D-F8'!$A$3</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">'WS2812D-F8'!$A$3:$A$6</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">'WS2812D-F8'!$A$4</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">'WS2812D-F8'!$A$5</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">'WS2812D-F8'!$A$6</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">'WS2812D-F8'!$B$2:$AK$2</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">'WS2812D-F8'!$B$2:$C$2</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">'WS2812D-F8'!$B$2:$J$2</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">'WS2812D-F8'!$B$3:$AK$3</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Wavelength!$A$9:$A$14</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">'WS2812D-F8'!$B$3:$C$3</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">'WS2812D-F8'!$B$3:$J$3</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">'WS2812D-F8'!$B$4:$AK$4</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">'WS2812D-F8'!$B$4:$C$4</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">'WS2812D-F8'!$B$4:$J$4</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">'WS2812D-F8'!$B$5:$AK$5</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">'WS2812D-F8'!$B$5:$C$5</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">'WS2812D-F8'!$B$5:$J$5</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">'WS2812D-F8'!$B$6:$AK$6</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">'WS2812D-F8'!$B$6:$J$6</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">Wavelength!$A$9:$A$26</definedName>
+    <definedName name="_xlchart.v1.80" hidden="1">'WS2812D-F8'!$A$2</definedName>
+    <definedName name="_xlchart.v1.81" hidden="1">'WS2812D-F8'!$A$2:$A$5</definedName>
+    <definedName name="_xlchart.v1.82" hidden="1">'WS2812D-F8'!$A$3</definedName>
+    <definedName name="_xlchart.v1.83" hidden="1">'WS2812D-F8'!$A$4</definedName>
+    <definedName name="_xlchart.v1.84" hidden="1">'WS2812D-F8'!$A$5</definedName>
+    <definedName name="_xlchart.v1.85" hidden="1">'WS2812D-F8'!$B$1:$E$1</definedName>
+    <definedName name="_xlchart.v1.86" hidden="1">'WS2812D-F8'!$B$1:$S$1</definedName>
+    <definedName name="_xlchart.v1.87" hidden="1">'WS2812D-F8'!$B$2:$E$2</definedName>
+    <definedName name="_xlchart.v1.88" hidden="1">'WS2812D-F8'!$B$2:$S$2</definedName>
+    <definedName name="_xlchart.v1.89" hidden="1">'WS2812D-F8'!$B$3:$E$3</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">Wavelength!$B$9:$B$14</definedName>
+    <definedName name="_xlchart.v1.90" hidden="1">'WS2812D-F8'!$B$3:$S$3</definedName>
+    <definedName name="_xlchart.v1.91" hidden="1">'WS2812D-F8'!$B$4:$E$4</definedName>
+    <definedName name="_xlchart.v1.92" hidden="1">'WS2812D-F8'!$B$4:$S$4</definedName>
+    <definedName name="_xlchart.v1.93" hidden="1">'WS2812D-F8'!$B$5:$E$5</definedName>
+    <definedName name="_xlchart.v1.94" hidden="1">'WS2812D-F8'!$B$5:$S$5</definedName>
+    <definedName name="_xlchart.v1.95" hidden="1">'WS2812D-F8'!#REF!</definedName>
+    <definedName name="_xlchart.v1.96" hidden="1">'WS2812D-F8'!$A$3</definedName>
+    <definedName name="_xlchart.v1.97" hidden="1">'WS2812D-F8'!$A$3:$A$6</definedName>
+    <definedName name="_xlchart.v1.98" hidden="1">'WS2812D-F8'!$A$4</definedName>
+    <definedName name="_xlchart.v1.99" hidden="1">'WS2812D-F8'!$A$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -81,6 +184,82 @@
   <si>
     <t>https://cdn-shop.adafruit.com/datasheets/TCS34725.pdf</t>
   </si>
+  <si>
+    <t>R-&gt;R</t>
+  </si>
+  <si>
+    <t>sensor 0</t>
+  </si>
+  <si>
+    <t>sensor 1</t>
+  </si>
+  <si>
+    <t>sensor 2</t>
+  </si>
+  <si>
+    <t>R-&gt;G</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>R-&gt;B</t>
+  </si>
+  <si>
+    <t>G-&gt;R</t>
+  </si>
+  <si>
+    <t>G-&gt;G</t>
+  </si>
+  <si>
+    <t>G-&gt;B</t>
+  </si>
+  <si>
+    <t>B-&gt;R</t>
+  </si>
+  <si>
+    <t>B-&gt;G</t>
+  </si>
+  <si>
+    <t>B-&gt;B</t>
+  </si>
+  <si>
+    <t>gain=2</t>
+  </si>
+  <si>
+    <t>gain=0 / TCS min</t>
+  </si>
+  <si>
+    <t>gain=1 / TCS max</t>
+  </si>
+  <si>
+    <t>actual value</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>measured:</t>
+  </si>
+  <si>
+    <t>measured value</t>
+  </si>
+  <si>
+    <t>actual
+value</t>
+  </si>
+  <si>
+    <t>TCS datasheet</t>
+  </si>
+  <si>
+    <t>avg values</t>
+  </si>
 </sst>
 </file>
 
@@ -111,7 +290,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -119,13 +298,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,6 +1101,218 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.66</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f dir="row">_xlchart.v1.69</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.66</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f dir="row">_xlchart.v1.72</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.66</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f dir="row">_xlchart.v1.75</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.66</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f dir="row">_xlchart.v1.78</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>WS2812 setting (R/G/B) to TCS color channels</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>WS2812 setting (R/G/B) to TCS color channels</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{C1DFF358-B924-4B3B-AA82-5849DEA317BA}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.61</cx:f>
+              <cx:v>TCS datasheet</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{DEA800AB-44B4-4915-B813-09307F44E629}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.63</cx:f>
+              <cx:v>sensor 0</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{ABC88451-4737-458D-8CF0-CB3B8667ED76}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.64</cx:f>
+              <cx:v>sensor 1</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+          </cx:spPr>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{27835B6F-07F2-42F0-AA9A-DC45B9305EA3}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.65</cx:f>
+              <cx:v>sensor 2</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>WS2812 value -&gt; measured value on color channel (R/G/B - red/green/blue)</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>WS2812 value -&gt; measured value on color channel (R/G/B - red/green/blue)</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Measured value on color channel relative to clear channel</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Measured value on color channel relative to clear channel</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+        <cx:numFmt formatCode="0%" sourceLinked="0"/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0">
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+          </a:endParaRPr>
+        </a:p>
+      </cx:txPr>
+    </cx:legend>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -992,6 +1433,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
@@ -2523,6 +3004,521 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2724,6 +3720,89 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D47F38D0-8131-4216-89D2-3323549AE667}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="257175" y="1557336"/>
+              <a:ext cx="10363200" cy="6577013"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3023,7 +4102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA8CF85-0C1B-482D-9D53-203BBD7DDB35}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
@@ -3386,4 +4465,702 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF689A4-10B4-41AC-AF04-292D4076C118}">
+  <dimension ref="A1:AK21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17:AD21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.140625" customWidth="1"/>
+    <col min="28" max="30" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>0.8</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.05</v>
+      </c>
+      <c r="E3">
+        <v>0.04</v>
+      </c>
+      <c r="F3">
+        <v>0.6</v>
+      </c>
+      <c r="G3">
+        <v>0.1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.1</v>
+      </c>
+      <c r="J3">
+        <v>0.65</v>
+      </c>
+      <c r="K3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M3">
+        <v>0.24</v>
+      </c>
+      <c r="N3">
+        <v>0.25</v>
+      </c>
+      <c r="O3">
+        <v>0.85</v>
+      </c>
+      <c r="P3">
+        <v>0.45</v>
+      </c>
+      <c r="Q3">
+        <v>0.15</v>
+      </c>
+      <c r="R3">
+        <v>0.42</v>
+      </c>
+      <c r="S3">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>0.93</v>
+      </c>
+      <c r="C4">
+        <v>0.04</v>
+      </c>
+      <c r="D4">
+        <v>0.09</v>
+      </c>
+      <c r="E4">
+        <v>0.09</v>
+      </c>
+      <c r="F4">
+        <v>0.63</v>
+      </c>
+      <c r="G4">
+        <v>0.25</v>
+      </c>
+      <c r="H4">
+        <v>0.01</v>
+      </c>
+      <c r="I4">
+        <v>0.22</v>
+      </c>
+      <c r="J4">
+        <v>0.78</v>
+      </c>
+      <c r="K4">
+        <v>0.92</v>
+      </c>
+      <c r="L4">
+        <v>0.04</v>
+      </c>
+      <c r="M4">
+        <v>0.09</v>
+      </c>
+      <c r="N4">
+        <v>0.09</v>
+      </c>
+      <c r="O4">
+        <v>0.63</v>
+      </c>
+      <c r="P4">
+        <v>0.24</v>
+      </c>
+      <c r="Q4">
+        <v>0.01</v>
+      </c>
+      <c r="R4">
+        <v>0.22</v>
+      </c>
+      <c r="S4">
+        <v>0.77</v>
+      </c>
+      <c r="T4">
+        <v>0.93</v>
+      </c>
+      <c r="U4">
+        <v>0.04</v>
+      </c>
+      <c r="V4">
+        <v>0.09</v>
+      </c>
+      <c r="W4">
+        <v>0.09</v>
+      </c>
+      <c r="X4">
+        <v>0.64</v>
+      </c>
+      <c r="Y4">
+        <v>0.25</v>
+      </c>
+      <c r="Z4">
+        <v>0.01</v>
+      </c>
+      <c r="AA4">
+        <v>0.22</v>
+      </c>
+      <c r="AB4">
+        <v>0.78</v>
+      </c>
+      <c r="AC4">
+        <v>0.92</v>
+      </c>
+      <c r="AD4">
+        <v>0.04</v>
+      </c>
+      <c r="AE4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AF4">
+        <v>0.09</v>
+      </c>
+      <c r="AG4">
+        <v>0.62</v>
+      </c>
+      <c r="AH4">
+        <v>0.22</v>
+      </c>
+      <c r="AI4">
+        <v>0.01</v>
+      </c>
+      <c r="AJ4">
+        <v>0.21</v>
+      </c>
+      <c r="AK4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0.88</v>
+      </c>
+      <c r="C5">
+        <v>0.06</v>
+      </c>
+      <c r="D5">
+        <v>0.09</v>
+      </c>
+      <c r="E5">
+        <v>0.09</v>
+      </c>
+      <c r="F5">
+        <v>0.66</v>
+      </c>
+      <c r="G5">
+        <v>0.27</v>
+      </c>
+      <c r="H5">
+        <v>0.01</v>
+      </c>
+      <c r="I5">
+        <v>0.25</v>
+      </c>
+      <c r="J5">
+        <v>0.79</v>
+      </c>
+      <c r="K5">
+        <v>0.88</v>
+      </c>
+      <c r="L5">
+        <v>0.06</v>
+      </c>
+      <c r="M5">
+        <v>0.09</v>
+      </c>
+      <c r="N5">
+        <v>0.09</v>
+      </c>
+      <c r="O5">
+        <v>0.67</v>
+      </c>
+      <c r="P5">
+        <v>0.27</v>
+      </c>
+      <c r="Q5">
+        <v>0.01</v>
+      </c>
+      <c r="R5">
+        <v>0.25</v>
+      </c>
+      <c r="S5">
+        <v>0.79</v>
+      </c>
+      <c r="T5">
+        <v>0.89</v>
+      </c>
+      <c r="U5">
+        <v>0.06</v>
+      </c>
+      <c r="V5">
+        <v>0.09</v>
+      </c>
+      <c r="W5">
+        <v>0.09</v>
+      </c>
+      <c r="X5">
+        <v>0.66</v>
+      </c>
+      <c r="Y5">
+        <v>0.27</v>
+      </c>
+      <c r="Z5">
+        <v>0.01</v>
+      </c>
+      <c r="AA5">
+        <v>0.25</v>
+      </c>
+      <c r="AB5">
+        <v>0.78</v>
+      </c>
+      <c r="AC5">
+        <v>0.9</v>
+      </c>
+      <c r="AD5">
+        <v>0.06</v>
+      </c>
+      <c r="AE5">
+        <v>0.09</v>
+      </c>
+      <c r="AF5">
+        <v>0.09</v>
+      </c>
+      <c r="AG5">
+        <v>0.66</v>
+      </c>
+      <c r="AH5">
+        <v>0.26</v>
+      </c>
+      <c r="AI5">
+        <v>0.01</v>
+      </c>
+      <c r="AJ5">
+        <v>0.25</v>
+      </c>
+      <c r="AK5">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>0.84</v>
+      </c>
+      <c r="C6">
+        <v>0.04</v>
+      </c>
+      <c r="D6">
+        <v>0.08</v>
+      </c>
+      <c r="E6">
+        <v>0.09</v>
+      </c>
+      <c r="F6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G6">
+        <v>0.22</v>
+      </c>
+      <c r="H6">
+        <v>0.01</v>
+      </c>
+      <c r="I6">
+        <v>0.2</v>
+      </c>
+      <c r="J6">
+        <v>0.65</v>
+      </c>
+      <c r="K6">
+        <v>0.84</v>
+      </c>
+      <c r="L6">
+        <v>0.04</v>
+      </c>
+      <c r="M6">
+        <v>0.08</v>
+      </c>
+      <c r="N6">
+        <v>0.09</v>
+      </c>
+      <c r="O6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P6">
+        <v>0.22</v>
+      </c>
+      <c r="Q6">
+        <v>0.01</v>
+      </c>
+      <c r="R6">
+        <v>0.19</v>
+      </c>
+      <c r="S6">
+        <v>0.66</v>
+      </c>
+      <c r="T6">
+        <v>0.84</v>
+      </c>
+      <c r="U6">
+        <v>0.04</v>
+      </c>
+      <c r="V6">
+        <v>0.08</v>
+      </c>
+      <c r="W6">
+        <v>0.09</v>
+      </c>
+      <c r="X6">
+        <v>0.54</v>
+      </c>
+      <c r="Y6">
+        <v>0.23</v>
+      </c>
+      <c r="Z6">
+        <v>0.01</v>
+      </c>
+      <c r="AA6">
+        <v>0.19</v>
+      </c>
+      <c r="AB6">
+        <v>0.66</v>
+      </c>
+      <c r="AC6">
+        <v>0.88</v>
+      </c>
+      <c r="AD6">
+        <v>0.06</v>
+      </c>
+      <c r="AE6">
+        <v>0.09</v>
+      </c>
+      <c r="AF6">
+        <v>0.08</v>
+      </c>
+      <c r="AG6">
+        <v>0.66</v>
+      </c>
+      <c r="AH6">
+        <v>0.25</v>
+      </c>
+      <c r="AI6">
+        <v>0.01</v>
+      </c>
+      <c r="AJ6">
+        <v>0.22</v>
+      </c>
+      <c r="AK6">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="17" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="U17" t="s">
+        <v>32</v>
+      </c>
+      <c r="V17" t="s">
+        <v>29</v>
+      </c>
+      <c r="W17" t="s">
+        <v>30</v>
+      </c>
+      <c r="X17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+    </row>
+    <row r="18" spans="20:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T18" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD18" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="20:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T19" t="s">
+        <v>29</v>
+      </c>
+      <c r="V19" t="str">
+        <f>_xlfn.CONCAT($T19, "-&gt;", V$17)</f>
+        <v>R-&gt;R</v>
+      </c>
+      <c r="W19" t="str">
+        <f t="shared" ref="W19:X19" si="0">_xlfn.CONCAT($T19, "-&gt;", W$17)</f>
+        <v>R-&gt;G</v>
+      </c>
+      <c r="X19" t="str">
+        <f t="shared" si="0"/>
+        <v>R-&gt;B</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB19" s="5">
+        <f>AVERAGEIF($2:$2, V19, $4:$6)</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="AC19" s="5">
+        <f>AVERAGEIF($2:$2, W19, $4:$6)</f>
+        <v>0.04</v>
+      </c>
+      <c r="AD19" s="5">
+        <f>AVERAGEIF($2:$2, X19, $4:$6)</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="20:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T20" t="s">
+        <v>30</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" ref="V20:X21" si="1">_xlfn.CONCAT($T20, "-&gt;", V$17)</f>
+        <v>G-&gt;R</v>
+      </c>
+      <c r="W20" t="str">
+        <f t="shared" si="1"/>
+        <v>G-&gt;G</v>
+      </c>
+      <c r="X20" t="str">
+        <f t="shared" si="1"/>
+        <v>G-&gt;B</v>
+      </c>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB20" s="5">
+        <f>AVERAGEIF($2:$2, V20, $4:$6)</f>
+        <v>0.09</v>
+      </c>
+      <c r="AC20" s="5">
+        <f>AVERAGEIF($2:$2, W20, $4:$6)</f>
+        <v>0.63</v>
+      </c>
+      <c r="AD20" s="5">
+        <f>AVERAGEIF($2:$2, X20, $4:$6)</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="21" spans="20:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T21" t="s">
+        <v>31</v>
+      </c>
+      <c r="V21" t="str">
+        <f t="shared" si="1"/>
+        <v>B-&gt;R</v>
+      </c>
+      <c r="W21" t="str">
+        <f t="shared" si="1"/>
+        <v>B-&gt;G</v>
+      </c>
+      <c r="X21" t="str">
+        <f t="shared" si="1"/>
+        <v>B-&gt;B</v>
+      </c>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB21" s="5">
+        <f>AVERAGEIF($2:$2, V21, $4:$6)</f>
+        <v>0.01</v>
+      </c>
+      <c r="AC21" s="5">
+        <f>AVERAGEIF($2:$2, W21, $4:$6)</f>
+        <v>0.2175</v>
+      </c>
+      <c r="AD21" s="5">
+        <f>AVERAGEIF($2:$2, X21, $4:$6)</f>
+        <v>0.77</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="Z19:Z21"/>
+    <mergeCell ref="AB17:AD17"/>
+  </mergeCells>
+  <conditionalFormatting sqref="AB19:AD21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>